<commit_message>
last update on 20/03/2023
</commit_message>
<xml_diff>
--- a/assets/files/student_form_data_update.xlsx
+++ b/assets/files/student_form_data_update.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/fieldwork_nuol/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE4A035-A63F-964B-9DA6-BE35272EE5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BDB04F-A407-8D4D-BBD9-6BC3F82E1305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20040" xr2:uid="{F46E6FF6-3060-2745-AE4A-2972A309CDBC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{F46E6FF6-3060-2745-AE4A-2972A309CDBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Student_data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ລ/ດ
 No</t>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>ຂໍ້ມູນນັກສຶກສາ ພາກວິຊາ ວິສະວະກໍາ ຄອມພິວເຕີ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -265,6 +268,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B1BD51-4EEA-FD47-881E-E9E03E50A70F}">
-  <dimension ref="A1:K2164"/>
+  <dimension ref="A1:K2165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -598,64 +605,66 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+    </row>
+    <row r="2" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-    </row>
-    <row r="2" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="15" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="10" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
@@ -28750,15 +28759,29 @@
       <c r="J2164" s="3"/>
       <c r="K2164" s="3"/>
     </row>
+    <row r="2165" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A2165" s="2"/>
+      <c r="B2165" s="3"/>
+      <c r="C2165" s="3"/>
+      <c r="D2165" s="3"/>
+      <c r="E2165" s="3"/>
+      <c r="F2165" s="3"/>
+      <c r="G2165" s="3"/>
+      <c r="H2165" s="11"/>
+      <c r="I2165" s="3"/>
+      <c r="J2165" s="3"/>
+      <c r="K2165" s="3"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="3">
-    <mergeCell ref="D2:E2"/>
+  <mergeCells count="4">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="date of birthday" error="ກະລຸນາປ້ອນວັນເດືອນປີເກີດເປັນ yyyy-mm-dd" sqref="H2163:H1048576" xr:uid="{BA794757-C150-E14B-9A9D-AC82E15A7EF1}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="date of birthday" error="ກະລຸນາປ້ອນວັນເດືອນປີເກີດເປັນ yyyy-mm-dd" sqref="H2164:H1048576" xr:uid="{BA794757-C150-E14B-9A9D-AC82E15A7EF1}">
       <formula1>36161</formula1>
       <formula2>TODAY()</formula2>
     </dataValidation>

</xml_diff>